<commit_message>
add bulk copy tool
</commit_message>
<xml_diff>
--- a/py/config.xlsx
+++ b/py/config.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dev\ICBC_E-Stamp_Tool\py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BD059A-17FE-403B-AC62-46647D348323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95E0A5C-38F1-4EFE-9F60-0E2D819583AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4170" yWindow="1365" windowWidth="21600" windowHeight="10335" xr2:uid="{3B349FB4-A0DD-4A60-A156-A5AD021FD122}"/>
+    <workbookView xWindow="-24360" yWindow="2475" windowWidth="21600" windowHeight="10335" activeTab="1" xr2:uid="{3B349FB4-A0DD-4A60-A156-A5AD021FD122}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ICBC E-Stamp Tool" sheetId="1" r:id="rId1"/>
+    <sheet name="Bulk Copy ICBC" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Producer Code</t>
   </si>
@@ -76,6 +77,18 @@
   </si>
   <si>
     <t>Echo</t>
+  </si>
+  <si>
+    <t>Input_Path</t>
+  </si>
+  <si>
+    <t>Onput_Path</t>
+  </si>
+  <si>
+    <t>C:\Users\&lt;USERNAME&gt;\Desktop\Old ICBC Copies</t>
+  </si>
+  <si>
+    <t>C:\Users\&lt;USERNAME&gt;\Desktop\New ICBC Copies</t>
   </si>
 </sst>
 </file>
@@ -455,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE055F9C-29E1-41D0-826E-64D35381AD11}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="A3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,4 +537,86 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EE59C6-8A0C-480C-80C9-5B3F6B46AF42}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>